<commit_message>
Updated Test Case 4
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111THEMIX00000/THEMIX_ITALIA_SRL/WLAB/126.2.c.a2/report-checklist.xlsx
+++ b/GATEWAY/S1#111THEMIX00000/THEMIX_ITALIA_SRL/WLAB/126.2.c.a2/report-checklist.xlsx
@@ -584,9 +584,6 @@
     <t>2023-02-24T14:59:17Z</t>
   </si>
   <si>
-    <t>2023-02-24T14:59:22Z</t>
-  </si>
-  <si>
     <t>2023-02-24T14:58:56Z</t>
   </si>
   <si>
@@ -599,9 +596,6 @@
     <t>b4cb9c81e4ac1673</t>
   </si>
   <si>
-    <t>be4e5297b988ef6b</t>
-  </si>
-  <si>
     <t>ec5937ec104b75da</t>
   </si>
   <si>
@@ -612,9 +606,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.844058695c9ddd088f3afdc4e917d64d482c293dd8036cae4e45ccf935df5fb4.ca84f797b0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.92eb3aeb202cab0e280ba955b9e2978f4b3c5003a6a717fd5501914d7a5e0a45.e7e34b1246^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.3b2e59a6e381b467f37b23357e2a786e0ccf04b205c4f4c85da19139115f84f0.db77382c73^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
@@ -684,6 +675,15 @@
   </si>
   <si>
     <t>2023-03-02T11:27:45Z</t>
+  </si>
+  <si>
+    <t>2023-03-06T13:07:40Z</t>
+  </si>
+  <si>
+    <t>9db1f31bed25ff1b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.e932cae83dd7f32d9bc74277861d37c63f6f1ca471070fe0523d9538f067b774.c9f81f2598^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2806,10 +2806,10 @@
   <dimension ref="A1:T873"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -3093,10 +3093,10 @@
         <v>110</v>
       </c>
       <c r="H10" s="40" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I10" s="40" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J10" s="41" t="s">
         <v>44</v>
@@ -3137,10 +3137,10 @@
         <v>111</v>
       </c>
       <c r="H11" s="40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I11" s="40" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J11" s="41" t="s">
         <v>44</v>
@@ -3181,10 +3181,10 @@
         <v>112</v>
       </c>
       <c r="H12" s="40" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I12" s="40" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J12" s="41" t="s">
         <v>44</v>
@@ -3219,16 +3219,16 @@
         <v>34</v>
       </c>
       <c r="F13" s="39">
-        <v>44981</v>
+        <v>44991</v>
       </c>
       <c r="G13" s="40" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="H13" s="40" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="I13" s="40" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="J13" s="41" t="s">
         <v>44</v>
@@ -3266,13 +3266,13 @@
         <v>44981</v>
       </c>
       <c r="G14" s="40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H14" s="40" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I14" s="40" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="J14" s="41" t="s">
         <v>44</v>
@@ -3314,7 +3314,7 @@
         <v>88</v>
       </c>
       <c r="K15" s="41" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="L15" s="41" t="s">
         <v>44</v>
@@ -3323,13 +3323,13 @@
         <v>44</v>
       </c>
       <c r="N15" s="41" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="O15" s="41" t="s">
         <v>88</v>
       </c>
       <c r="P15" s="41" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="Q15" s="41"/>
       <c r="R15" s="44"/>
@@ -3358,13 +3358,13 @@
         <v>44981</v>
       </c>
       <c r="G16" s="40" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H16" s="40" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I16" s="40" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="J16" s="41" t="s">
         <v>44</v>
@@ -3377,13 +3377,13 @@
         <v>44</v>
       </c>
       <c r="N16" s="41" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="O16" s="41" t="s">
         <v>44</v>
       </c>
       <c r="P16" s="41" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="Q16" s="41"/>
       <c r="R16" s="44"/>
@@ -3413,7 +3413,7 @@
       <c r="H17" s="40"/>
       <c r="I17" s="40"/>
       <c r="J17" s="41" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K17" s="41"/>
       <c r="L17" s="41" t="s">
@@ -3423,13 +3423,13 @@
         <v>44</v>
       </c>
       <c r="N17" s="41" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="O17" s="41" t="s">
         <v>88</v>
       </c>
       <c r="P17" s="41" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Q17" s="41"/>
       <c r="R17" s="44" t="s">
@@ -3464,7 +3464,7 @@
         <v>88</v>
       </c>
       <c r="K18" s="41" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="L18" s="41" t="s">
         <v>44</v>
@@ -3504,7 +3504,7 @@
         <v>88</v>
       </c>
       <c r="K19" s="41" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L19" s="41"/>
       <c r="M19" s="41"/>
@@ -3542,7 +3542,7 @@
         <v>88</v>
       </c>
       <c r="K20" s="41" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L20" s="41"/>
       <c r="M20" s="41"/>
@@ -3580,7 +3580,7 @@
         <v>88</v>
       </c>
       <c r="K21" s="48" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L21" s="41" t="s">
         <v>88</v>
@@ -3624,7 +3624,7 @@
         <v>88</v>
       </c>
       <c r="K22" s="41" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="L22" s="41" t="s">
         <v>44</v>
@@ -3664,7 +3664,7 @@
         <v>88</v>
       </c>
       <c r="K23" s="41" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="L23" s="41"/>
       <c r="M23" s="41"/>
@@ -3702,7 +3702,7 @@
         <v>88</v>
       </c>
       <c r="K24" s="41" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="L24" s="41"/>
       <c r="M24" s="41"/>
@@ -3740,7 +3740,7 @@
         <v>88</v>
       </c>
       <c r="K25" s="41" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="L25" s="41"/>
       <c r="M25" s="41"/>
@@ -3778,7 +3778,7 @@
         <v>88</v>
       </c>
       <c r="K26" s="41" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="L26" s="41"/>
       <c r="M26" s="41"/>
@@ -3816,7 +3816,7 @@
         <v>88</v>
       </c>
       <c r="K27" s="41" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="L27" s="41"/>
       <c r="M27" s="41"/>
@@ -3854,7 +3854,7 @@
         <v>88</v>
       </c>
       <c r="K28" s="41" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="L28" s="41"/>
       <c r="M28" s="41"/>
@@ -20434,6 +20434,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -20664,27 +20684,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6395DAD-5B77-46ED-9147-4C5A384B6E5B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20701,29 +20726,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Aggiunti a report-checklist.xlsx i casi 191 e 376
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111THEMIX00000/THEMIX_ITALIA_SRL/WLAB/126.2.c.a2/report-checklist.xlsx
+++ b/GATEWAY/S1#111THEMIX00000/THEMIX_ITALIA_SRL/WLAB/126.2.c.a2/report-checklist.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2275" uniqueCount="915">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2279" uniqueCount="916">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4765,6 +4765,9 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4628c463c305eb4930ba71fa1d0e1e442cfd01b1768c71999c5ee1914d3d155f.be50bc3f03^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Il nostro gestionale non si occupa del trasfusionale</t>
   </si>
 </sst>
 </file>
@@ -7689,10 +7692,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="D198" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I381" sqref="I381"/>
+      <selection pane="bottomRight" activeCell="K198" sqref="K198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -14745,7 +14748,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="198" spans="1:20" ht="150.75" thickBot="1">
       <c r="A198" s="20">
         <v>191</v>
       </c>
@@ -14765,8 +14768,12 @@
       <c r="G198" s="24"/>
       <c r="H198" s="24"/>
       <c r="I198" s="24"/>
-      <c r="J198" s="25"/>
-      <c r="K198" s="25"/>
+      <c r="J198" s="25" t="s">
+        <v>848</v>
+      </c>
+      <c r="K198" s="25" t="s">
+        <v>915</v>
+      </c>
       <c r="L198" s="25"/>
       <c r="M198" s="25"/>
       <c r="N198" s="25"/>
@@ -20987,7 +20994,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="381" spans="1:20" ht="165">
+    <row r="381" spans="1:20" ht="165.75" thickBot="1">
       <c r="A381" s="20">
         <v>374</v>
       </c>
@@ -21031,7 +21038,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="382" spans="1:20" ht="165" hidden="1">
+    <row r="382" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A382" s="20">
         <v>375</v>
       </c>
@@ -21065,7 +21072,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="383" spans="1:20" ht="165" hidden="1">
+    <row r="383" spans="1:20" ht="165">
       <c r="A383" s="20">
         <v>376</v>
       </c>
@@ -21085,8 +21092,12 @@
       <c r="G383" s="24"/>
       <c r="H383" s="24"/>
       <c r="I383" s="24"/>
-      <c r="J383" s="25"/>
-      <c r="K383" s="25"/>
+      <c r="J383" s="25" t="s">
+        <v>848</v>
+      </c>
+      <c r="K383" s="25" t="s">
+        <v>915</v>
+      </c>
       <c r="L383" s="25"/>
       <c r="M383" s="25"/>
       <c r="N383" s="25"/>
@@ -25752,90 +25763,19 @@
     </row>
   </sheetData>
   <autoFilter ref="A9:T383">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="1"/>
-        <filter val="11"/>
-        <filter val="12"/>
-        <filter val="13"/>
-        <filter val="14"/>
-        <filter val="147"/>
-        <filter val="148"/>
-        <filter val="149"/>
-        <filter val="150"/>
-        <filter val="151"/>
-        <filter val="152"/>
-        <filter val="153"/>
-        <filter val="154"/>
-        <filter val="155"/>
-        <filter val="156"/>
-        <filter val="157"/>
-        <filter val="158"/>
-        <filter val="159"/>
-        <filter val="160"/>
-        <filter val="161"/>
-        <filter val="162"/>
-        <filter val="163"/>
-        <filter val="164"/>
-        <filter val="165"/>
-        <filter val="166"/>
-        <filter val="167"/>
-        <filter val="168"/>
-        <filter val="169"/>
-        <filter val="2"/>
-        <filter val="28"/>
-        <filter val="3"/>
-        <filter val="31"/>
-        <filter val="32"/>
-        <filter val="36"/>
-        <filter val="368"/>
-        <filter val="370"/>
-        <filter val="374"/>
-        <filter val="39"/>
-        <filter val="4"/>
-        <filter val="40"/>
-        <filter val="44"/>
-        <filter val="47"/>
-        <filter val="48"/>
-        <filter val="5"/>
-        <filter val="52"/>
-        <filter val="53"/>
-        <filter val="54"/>
-        <filter val="55"/>
-        <filter val="56"/>
-        <filter val="57"/>
-        <filter val="58"/>
-        <filter val="59"/>
-        <filter val="60"/>
-        <filter val="61"/>
-        <filter val="62"/>
-        <filter val="75"/>
-        <filter val="76"/>
-        <filter val="77"/>
-        <filter val="78"/>
-        <filter val="79"/>
-        <filter val="80"/>
-        <filter val="81"/>
-        <filter val="82"/>
-        <filter val="83"/>
-        <filter val="84"/>
-        <filter val="85"/>
-        <filter val="86"/>
-        <filter val="87"/>
-        <filter val="88"/>
-        <filter val="89"/>
-        <filter val="90"/>
-        <filter val="91"/>
-        <filter val="92"/>
-        <filter val="93"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="0"/>
     <filterColumn colId="1">
       <filters>
         <filter val="VALIDAZIONE"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="2"/>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="LAB"/>
+        <filter val="RAD"/>
+        <filter val="RSA"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="9"/>
   </autoFilter>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Reupload casi test 1,2,3,4,5 e 36
commonName auth: S1#111THEMIX00000
subject_application_vendor: THEMIX ITALIA SRL
subject_application_id: WLAB
subject_application_version: 126.2.c.a2
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111THEMIX00000/THEMIX_ITALIA_SRL/WLAB/126.2.c.a2/report-checklist.xlsx
+++ b/GATEWAY/S1#111THEMIX00000/THEMIX_ITALIA_SRL/WLAB/126.2.c.a2/report-checklist.xlsx
@@ -4581,60 +4581,9 @@
     <t>subject_application_version: 126.2.c.a2</t>
   </si>
   <si>
-    <t>2023-02-24T14:58:18Z</t>
-  </si>
-  <si>
-    <t>af2db383a0a623e8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.533d3b742b1ab4a78b2922b599b076f69eba5c906f92ac70aaf5118410dd4976.4197ac9da5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-24T14:59:10Z</t>
-  </si>
-  <si>
-    <t>65de55431999c4d3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.7d7c6b2a7b88db6a7be3d795555a081663158b6cdcabf5459d6f77630716de94.05d6a91b53^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-24T14:59:17Z</t>
-  </si>
-  <si>
-    <t>b4cb9c81e4ac1673</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.844058695c9ddd088f3afdc4e917d64d482c293dd8036cae4e45ccf935df5fb4.ca84f797b0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-06T13:07:40Z</t>
-  </si>
-  <si>
-    <t>9db1f31bed25ff1b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.e932cae83dd7f32d9bc74277861d37c63f6f1ca471070fe0523d9538f067b774.c9f81f2598^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-24T14:58:56Z</t>
-  </si>
-  <si>
-    <t>ec5937ec104b75da</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.3b2e59a6e381b467f37b23357e2a786e0ccf04b205c4f4c85da19139115f84f0.db77382c73^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>La nostra libreria effettua un controllo sui dati che vengono passati per comporre il token, qualora ci fossero dati obbligatori mancanti il programma non effettua la chiamata al gateway ma ritorna un messaggio di errore informando l'utente che nella configurazione mancano dei dati obbligatori</t>
   </si>
   <si>
-    <t>2023-03-02T11:27:45Z</t>
-  </si>
-  <si>
-    <t>a9e93430e62a7f31</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
@@ -4768,6 +4717,57 @@
   </si>
   <si>
     <t>Il nostro gestionale non si occupa del trasfusionale</t>
+  </si>
+  <si>
+    <t>2023-12-12T08:54:33Z</t>
+  </si>
+  <si>
+    <t>8b926e7f6b8f8f6e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.533d3b742b1ab4a78b2922b599b076f69eba5c906f92ac70aaf5118410dd4976.933094d7e5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-12-12T08:56:53Z</t>
+  </si>
+  <si>
+    <t>a769a9d3363e0f85</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.7d7c6b2a7b88db6a7be3d795555a081663158b6cdcabf5459d6f77630716de94.78dc6d2306^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-12-12T09:31:48Z</t>
+  </si>
+  <si>
+    <t>1a9b0c7f305951c4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.844058695c9ddd088f3afdc4e917d64d482c293dd8036cae4e45ccf935df5fb4.551becac4f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-12-12T09:33:29Z</t>
+  </si>
+  <si>
+    <t>cb26e25ad6dd6f34</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.e932cae83dd7f32d9bc74277861d37c63f6f1ca471070fe0523d9538f067b774.2b63a973fd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-12-12T09:38:15Z</t>
+  </si>
+  <si>
+    <t>b637ca4c190f3a20</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.3b2e59a6e381b467f37b23357e2a786e0ccf04b205c4f4c85da19139115f84f0.e18db590bd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-12-12T09:43:32Z</t>
+  </si>
+  <si>
+    <t>cce8770dd437aa60</t>
   </si>
 </sst>
 </file>
@@ -7692,10 +7692,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D198" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="K198" sqref="K198"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -7965,16 +7965,16 @@
         <v>47</v>
       </c>
       <c r="F10" s="34">
-        <v>44981</v>
+        <v>45272</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>853</v>
+        <v>899</v>
       </c>
       <c r="H10" s="35" t="s">
-        <v>854</v>
+        <v>900</v>
       </c>
       <c r="I10" s="35" t="s">
-        <v>855</v>
+        <v>901</v>
       </c>
       <c r="J10" s="36" t="s">
         <v>139</v>
@@ -8009,16 +8009,16 @@
         <v>50</v>
       </c>
       <c r="F11" s="34">
-        <v>44981</v>
+        <v>45272</v>
       </c>
       <c r="G11" s="35" t="s">
-        <v>856</v>
+        <v>902</v>
       </c>
       <c r="H11" s="35" t="s">
-        <v>857</v>
+        <v>903</v>
       </c>
       <c r="I11" s="35" t="s">
-        <v>858</v>
+        <v>904</v>
       </c>
       <c r="J11" s="36" t="s">
         <v>139</v>
@@ -8053,16 +8053,16 @@
         <v>52</v>
       </c>
       <c r="F12" s="34">
-        <v>44981</v>
+        <v>45272</v>
       </c>
       <c r="G12" s="35" t="s">
-        <v>859</v>
+        <v>905</v>
       </c>
       <c r="H12" s="35" t="s">
-        <v>860</v>
+        <v>906</v>
       </c>
       <c r="I12" s="35" t="s">
-        <v>861</v>
+        <v>907</v>
       </c>
       <c r="J12" s="36" t="s">
         <v>139</v>
@@ -8097,16 +8097,16 @@
         <v>54</v>
       </c>
       <c r="F13" s="34">
-        <v>44991</v>
+        <v>45272</v>
       </c>
       <c r="G13" s="35" t="s">
-        <v>862</v>
+        <v>908</v>
       </c>
       <c r="H13" s="35" t="s">
-        <v>863</v>
+        <v>909</v>
       </c>
       <c r="I13" s="35" t="s">
-        <v>864</v>
+        <v>910</v>
       </c>
       <c r="J13" s="36" t="s">
         <v>139</v>
@@ -8141,16 +8141,16 @@
         <v>56</v>
       </c>
       <c r="F14" s="34">
-        <v>44981</v>
+        <v>45272</v>
       </c>
       <c r="G14" s="35" t="s">
-        <v>865</v>
+        <v>911</v>
       </c>
       <c r="H14" s="35" t="s">
-        <v>866</v>
+        <v>912</v>
       </c>
       <c r="I14" s="35" t="s">
-        <v>867</v>
+        <v>913</v>
       </c>
       <c r="J14" s="36" t="s">
         <v>139</v>
@@ -8324,13 +8324,13 @@
         <v>45265</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>906</v>
+        <v>889</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>904</v>
+        <v>887</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>905</v>
+        <v>888</v>
       </c>
       <c r="J19" s="25" t="s">
         <v>139</v>
@@ -8372,7 +8372,7 @@
         <v>848</v>
       </c>
       <c r="K20" s="25" t="s">
-        <v>887</v>
+        <v>870</v>
       </c>
       <c r="L20" s="25"/>
       <c r="M20" s="25"/>
@@ -8410,7 +8410,7 @@
         <v>848</v>
       </c>
       <c r="K21" s="25" t="s">
-        <v>888</v>
+        <v>871</v>
       </c>
       <c r="L21" s="25"/>
       <c r="M21" s="25"/>
@@ -8448,7 +8448,7 @@
         <v>848</v>
       </c>
       <c r="K22" s="25" t="s">
-        <v>888</v>
+        <v>871</v>
       </c>
       <c r="L22" s="25"/>
       <c r="M22" s="25"/>
@@ -8894,7 +8894,7 @@
         <v>848</v>
       </c>
       <c r="K35" s="36" t="s">
-        <v>868</v>
+        <v>853</v>
       </c>
       <c r="L35" s="36"/>
       <c r="M35" s="36"/>
@@ -9000,7 +9000,7 @@
         <v>848</v>
       </c>
       <c r="K38" s="36" t="s">
-        <v>868</v>
+        <v>853</v>
       </c>
       <c r="L38" s="25"/>
       <c r="M38" s="25"/>
@@ -9038,7 +9038,7 @@
         <v>848</v>
       </c>
       <c r="K39" s="36" t="s">
-        <v>868</v>
+        <v>853</v>
       </c>
       <c r="L39" s="25"/>
       <c r="M39" s="25"/>
@@ -9171,16 +9171,16 @@
         <v>122</v>
       </c>
       <c r="F43" s="34">
-        <v>44987</v>
+        <v>45272</v>
       </c>
       <c r="G43" s="35" t="s">
-        <v>869</v>
+        <v>914</v>
       </c>
       <c r="H43" s="35" t="s">
-        <v>870</v>
+        <v>915</v>
       </c>
       <c r="I43" s="35" t="s">
-        <v>871</v>
+        <v>854</v>
       </c>
       <c r="J43" s="36" t="s">
         <v>139</v>
@@ -9193,13 +9193,13 @@
         <v>139</v>
       </c>
       <c r="N43" s="36" t="s">
-        <v>872</v>
+        <v>855</v>
       </c>
       <c r="O43" s="36" t="s">
         <v>139</v>
       </c>
       <c r="P43" s="36" t="s">
-        <v>873</v>
+        <v>856</v>
       </c>
       <c r="Q43" s="25"/>
       <c r="R43" s="26"/>
@@ -9296,13 +9296,13 @@
         <v>45265</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>907</v>
+        <v>890</v>
       </c>
       <c r="H46" s="24" t="s">
-        <v>899</v>
+        <v>882</v>
       </c>
       <c r="I46" s="24" t="s">
-        <v>871</v>
+        <v>854</v>
       </c>
       <c r="J46" s="25" t="s">
         <v>139</v>
@@ -9315,13 +9315,13 @@
         <v>139</v>
       </c>
       <c r="N46" s="36" t="s">
-        <v>872</v>
+        <v>855</v>
       </c>
       <c r="O46" s="36" t="s">
         <v>139</v>
       </c>
       <c r="P46" s="36" t="s">
-        <v>873</v>
+        <v>856</v>
       </c>
       <c r="Q46" s="25"/>
       <c r="R46" s="26"/>
@@ -9350,13 +9350,13 @@
         <v>45266</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>910</v>
+        <v>893</v>
       </c>
       <c r="H47" s="24" t="s">
-        <v>911</v>
+        <v>894</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>871</v>
+        <v>854</v>
       </c>
       <c r="J47" s="25" t="s">
         <v>139</v>
@@ -9369,13 +9369,13 @@
         <v>139</v>
       </c>
       <c r="N47" s="36" t="s">
-        <v>872</v>
+        <v>855</v>
       </c>
       <c r="O47" s="36" t="s">
         <v>139</v>
       </c>
       <c r="P47" s="36" t="s">
-        <v>873</v>
+        <v>856</v>
       </c>
       <c r="Q47" s="25"/>
       <c r="R47" s="26"/>
@@ -9507,7 +9507,7 @@
       <c r="H51" s="24"/>
       <c r="I51" s="24"/>
       <c r="J51" s="36" t="s">
-        <v>874</v>
+        <v>857</v>
       </c>
       <c r="K51" s="36"/>
       <c r="L51" s="36" t="s">
@@ -9517,13 +9517,13 @@
         <v>139</v>
       </c>
       <c r="N51" s="36" t="s">
-        <v>875</v>
+        <v>858</v>
       </c>
       <c r="O51" s="36" t="s">
         <v>848</v>
       </c>
       <c r="P51" s="36" t="s">
-        <v>876</v>
+        <v>859</v>
       </c>
       <c r="Q51" s="25"/>
       <c r="R51" s="26" t="s">
@@ -9627,7 +9627,7 @@
       <c r="H54" s="24"/>
       <c r="I54" s="24"/>
       <c r="J54" s="36" t="s">
-        <v>874</v>
+        <v>857</v>
       </c>
       <c r="K54" s="25"/>
       <c r="L54" s="36" t="s">
@@ -9637,13 +9637,13 @@
         <v>139</v>
       </c>
       <c r="N54" s="36" t="s">
-        <v>875</v>
+        <v>858</v>
       </c>
       <c r="O54" s="36" t="s">
         <v>848</v>
       </c>
       <c r="P54" s="36" t="s">
-        <v>876</v>
+        <v>859</v>
       </c>
       <c r="Q54" s="25"/>
       <c r="R54" s="26" t="s">
@@ -9675,7 +9675,7 @@
       <c r="H55" s="24"/>
       <c r="I55" s="24"/>
       <c r="J55" s="36" t="s">
-        <v>874</v>
+        <v>857</v>
       </c>
       <c r="K55" s="25"/>
       <c r="L55" s="36" t="s">
@@ -9685,13 +9685,13 @@
         <v>139</v>
       </c>
       <c r="N55" s="36" t="s">
-        <v>875</v>
+        <v>858</v>
       </c>
       <c r="O55" s="36" t="s">
         <v>848</v>
       </c>
       <c r="P55" s="36" t="s">
-        <v>876</v>
+        <v>859</v>
       </c>
       <c r="Q55" s="25"/>
       <c r="R55" s="26" t="s">
@@ -9834,7 +9834,7 @@
         <v>848</v>
       </c>
       <c r="K59" s="36" t="s">
-        <v>889</v>
+        <v>872</v>
       </c>
       <c r="L59" s="36"/>
       <c r="M59" s="36"/>
@@ -9872,7 +9872,7 @@
         <v>848</v>
       </c>
       <c r="K60" s="36" t="s">
-        <v>877</v>
+        <v>860</v>
       </c>
       <c r="L60" s="36"/>
       <c r="M60" s="36"/>
@@ -9910,7 +9910,7 @@
         <v>848</v>
       </c>
       <c r="K61" s="36" t="s">
-        <v>878</v>
+        <v>861</v>
       </c>
       <c r="L61" s="36"/>
       <c r="M61" s="36"/>
@@ -9948,7 +9948,7 @@
         <v>848</v>
       </c>
       <c r="K62" s="37" t="s">
-        <v>879</v>
+        <v>862</v>
       </c>
       <c r="L62" s="36"/>
       <c r="M62" s="37"/>
@@ -9986,7 +9986,7 @@
         <v>848</v>
       </c>
       <c r="K63" s="36" t="s">
-        <v>880</v>
+        <v>863</v>
       </c>
       <c r="L63" s="36"/>
       <c r="M63" s="36"/>
@@ -10024,7 +10024,7 @@
         <v>848</v>
       </c>
       <c r="K64" s="36" t="s">
-        <v>881</v>
+        <v>864</v>
       </c>
       <c r="L64" s="36"/>
       <c r="M64" s="36"/>
@@ -10062,7 +10062,7 @@
         <v>848</v>
       </c>
       <c r="K65" s="36" t="s">
-        <v>882</v>
+        <v>865</v>
       </c>
       <c r="L65" s="36"/>
       <c r="M65" s="36"/>
@@ -10100,7 +10100,7 @@
         <v>848</v>
       </c>
       <c r="K66" s="36" t="s">
-        <v>883</v>
+        <v>866</v>
       </c>
       <c r="L66" s="36"/>
       <c r="M66" s="36"/>
@@ -10138,7 +10138,7 @@
         <v>848</v>
       </c>
       <c r="K67" s="36" t="s">
-        <v>884</v>
+        <v>867</v>
       </c>
       <c r="L67" s="36"/>
       <c r="M67" s="36"/>
@@ -10176,7 +10176,7 @@
         <v>848</v>
       </c>
       <c r="K68" s="36" t="s">
-        <v>885</v>
+        <v>868</v>
       </c>
       <c r="L68" s="36"/>
       <c r="M68" s="36"/>
@@ -10214,7 +10214,7 @@
         <v>848</v>
       </c>
       <c r="K69" s="36" t="s">
-        <v>886</v>
+        <v>869</v>
       </c>
       <c r="L69" s="36"/>
       <c r="M69" s="36"/>
@@ -10660,7 +10660,7 @@
         <v>848</v>
       </c>
       <c r="K82" s="36" t="s">
-        <v>889</v>
+        <v>872</v>
       </c>
       <c r="L82" s="25"/>
       <c r="M82" s="25"/>
@@ -10698,7 +10698,7 @@
         <v>848</v>
       </c>
       <c r="K83" s="36" t="s">
-        <v>877</v>
+        <v>860</v>
       </c>
       <c r="L83" s="25"/>
       <c r="M83" s="25"/>
@@ -10736,7 +10736,7 @@
         <v>848</v>
       </c>
       <c r="K84" s="36" t="s">
-        <v>878</v>
+        <v>861</v>
       </c>
       <c r="L84" s="25"/>
       <c r="M84" s="25"/>
@@ -10774,7 +10774,7 @@
         <v>848</v>
       </c>
       <c r="K85" s="37" t="s">
-        <v>879</v>
+        <v>862</v>
       </c>
       <c r="L85" s="25"/>
       <c r="M85" s="25"/>
@@ -10812,7 +10812,7 @@
         <v>848</v>
       </c>
       <c r="K86" s="36" t="s">
-        <v>880</v>
+        <v>863</v>
       </c>
       <c r="L86" s="25"/>
       <c r="M86" s="25"/>
@@ -10850,7 +10850,7 @@
         <v>848</v>
       </c>
       <c r="K87" s="36" t="s">
-        <v>881</v>
+        <v>864</v>
       </c>
       <c r="L87" s="25"/>
       <c r="M87" s="25"/>
@@ -10888,7 +10888,7 @@
         <v>848</v>
       </c>
       <c r="K88" s="25" t="s">
-        <v>894</v>
+        <v>877</v>
       </c>
       <c r="L88" s="25"/>
       <c r="M88" s="25"/>
@@ -10926,7 +10926,7 @@
         <v>848</v>
       </c>
       <c r="K89" s="36" t="s">
-        <v>882</v>
+        <v>865</v>
       </c>
       <c r="L89" s="25"/>
       <c r="M89" s="25"/>
@@ -10964,7 +10964,7 @@
         <v>848</v>
       </c>
       <c r="K90" s="36" t="s">
-        <v>883</v>
+        <v>866</v>
       </c>
       <c r="L90" s="25"/>
       <c r="M90" s="25"/>
@@ -11002,7 +11002,7 @@
         <v>848</v>
       </c>
       <c r="K91" s="25" t="s">
-        <v>890</v>
+        <v>873</v>
       </c>
       <c r="L91" s="25"/>
       <c r="M91" s="25"/>
@@ -11040,7 +11040,7 @@
         <v>848</v>
       </c>
       <c r="K92" s="25" t="s">
-        <v>891</v>
+        <v>874</v>
       </c>
       <c r="L92" s="25"/>
       <c r="M92" s="25"/>
@@ -11078,7 +11078,7 @@
         <v>848</v>
       </c>
       <c r="K93" s="25" t="s">
-        <v>892</v>
+        <v>875</v>
       </c>
       <c r="L93" s="25"/>
       <c r="M93" s="25"/>
@@ -11116,7 +11116,7 @@
         <v>848</v>
       </c>
       <c r="K94" s="25" t="s">
-        <v>898</v>
+        <v>881</v>
       </c>
       <c r="L94" s="25"/>
       <c r="M94" s="25"/>
@@ -11154,7 +11154,7 @@
         <v>848</v>
       </c>
       <c r="K95" s="25" t="s">
-        <v>892</v>
+        <v>875</v>
       </c>
       <c r="L95" s="25"/>
       <c r="M95" s="25"/>
@@ -11192,7 +11192,7 @@
         <v>848</v>
       </c>
       <c r="K96" s="25" t="s">
-        <v>892</v>
+        <v>875</v>
       </c>
       <c r="L96" s="25"/>
       <c r="M96" s="25"/>
@@ -11230,7 +11230,7 @@
         <v>848</v>
       </c>
       <c r="K97" s="25" t="s">
-        <v>892</v>
+        <v>875</v>
       </c>
       <c r="L97" s="25"/>
       <c r="M97" s="25"/>
@@ -11268,7 +11268,7 @@
         <v>848</v>
       </c>
       <c r="K98" s="25" t="s">
-        <v>892</v>
+        <v>875</v>
       </c>
       <c r="L98" s="25"/>
       <c r="M98" s="25"/>
@@ -11306,7 +11306,7 @@
         <v>848</v>
       </c>
       <c r="K99" s="25" t="s">
-        <v>892</v>
+        <v>875</v>
       </c>
       <c r="L99" s="25"/>
       <c r="M99" s="25"/>
@@ -11344,7 +11344,7 @@
         <v>848</v>
       </c>
       <c r="K100" s="25" t="s">
-        <v>893</v>
+        <v>876</v>
       </c>
       <c r="L100" s="25"/>
       <c r="M100" s="25"/>
@@ -13184,7 +13184,7 @@
         <v>848</v>
       </c>
       <c r="K154" s="25" t="s">
-        <v>888</v>
+        <v>871</v>
       </c>
       <c r="L154" s="25"/>
       <c r="M154" s="25"/>
@@ -13222,7 +13222,7 @@
         <v>848</v>
       </c>
       <c r="K155" s="25" t="s">
-        <v>888</v>
+        <v>871</v>
       </c>
       <c r="L155" s="25"/>
       <c r="M155" s="25"/>
@@ -13260,7 +13260,7 @@
         <v>848</v>
       </c>
       <c r="K156" s="25" t="s">
-        <v>888</v>
+        <v>871</v>
       </c>
       <c r="L156" s="25"/>
       <c r="M156" s="25"/>
@@ -13298,7 +13298,7 @@
         <v>848</v>
       </c>
       <c r="K157" s="25" t="s">
-        <v>888</v>
+        <v>871</v>
       </c>
       <c r="L157" s="25"/>
       <c r="M157" s="25"/>
@@ -13336,7 +13336,7 @@
         <v>848</v>
       </c>
       <c r="K158" s="36" t="s">
-        <v>889</v>
+        <v>872</v>
       </c>
       <c r="L158" s="25"/>
       <c r="M158" s="25"/>
@@ -13374,7 +13374,7 @@
         <v>848</v>
       </c>
       <c r="K159" s="36" t="s">
-        <v>877</v>
+        <v>860</v>
       </c>
       <c r="L159" s="25"/>
       <c r="M159" s="25"/>
@@ -13412,7 +13412,7 @@
         <v>848</v>
       </c>
       <c r="K160" s="36" t="s">
-        <v>878</v>
+        <v>861</v>
       </c>
       <c r="L160" s="25"/>
       <c r="M160" s="25"/>
@@ -13450,7 +13450,7 @@
         <v>848</v>
       </c>
       <c r="K161" s="37" t="s">
-        <v>879</v>
+        <v>862</v>
       </c>
       <c r="L161" s="25"/>
       <c r="M161" s="25"/>
@@ -13488,7 +13488,7 @@
         <v>848</v>
       </c>
       <c r="K162" s="36" t="s">
-        <v>880</v>
+        <v>863</v>
       </c>
       <c r="L162" s="25"/>
       <c r="M162" s="25"/>
@@ -13526,7 +13526,7 @@
         <v>848</v>
       </c>
       <c r="K163" s="36" t="s">
-        <v>881</v>
+        <v>864</v>
       </c>
       <c r="L163" s="25"/>
       <c r="M163" s="25"/>
@@ -13564,7 +13564,7 @@
         <v>848</v>
       </c>
       <c r="K164" s="25" t="s">
-        <v>897</v>
+        <v>880</v>
       </c>
       <c r="L164" s="25"/>
       <c r="M164" s="25"/>
@@ -13602,7 +13602,7 @@
         <v>848</v>
       </c>
       <c r="K165" s="36" t="s">
-        <v>882</v>
+        <v>865</v>
       </c>
       <c r="L165" s="25"/>
       <c r="M165" s="25"/>
@@ -13640,7 +13640,7 @@
         <v>848</v>
       </c>
       <c r="K166" s="36" t="s">
-        <v>883</v>
+        <v>866</v>
       </c>
       <c r="L166" s="25"/>
       <c r="M166" s="25"/>
@@ -13678,7 +13678,7 @@
         <v>848</v>
       </c>
       <c r="K167" s="25" t="s">
-        <v>895</v>
+        <v>878</v>
       </c>
       <c r="L167" s="25"/>
       <c r="M167" s="25"/>
@@ -13716,7 +13716,7 @@
         <v>848</v>
       </c>
       <c r="K168" s="25" t="s">
-        <v>891</v>
+        <v>874</v>
       </c>
       <c r="L168" s="25"/>
       <c r="M168" s="25"/>
@@ -13754,7 +13754,7 @@
         <v>848</v>
       </c>
       <c r="K169" s="25" t="s">
-        <v>892</v>
+        <v>875</v>
       </c>
       <c r="L169" s="25"/>
       <c r="M169" s="25"/>
@@ -13792,7 +13792,7 @@
         <v>848</v>
       </c>
       <c r="K170" s="25" t="s">
-        <v>898</v>
+        <v>881</v>
       </c>
       <c r="L170" s="25"/>
       <c r="M170" s="25"/>
@@ -13830,7 +13830,7 @@
         <v>848</v>
       </c>
       <c r="K171" s="25" t="s">
-        <v>892</v>
+        <v>875</v>
       </c>
       <c r="L171" s="25"/>
       <c r="M171" s="25"/>
@@ -13868,7 +13868,7 @@
         <v>848</v>
       </c>
       <c r="K172" s="25" t="s">
-        <v>892</v>
+        <v>875</v>
       </c>
       <c r="L172" s="25"/>
       <c r="M172" s="25"/>
@@ -13906,7 +13906,7 @@
         <v>848</v>
       </c>
       <c r="K173" s="25" t="s">
-        <v>892</v>
+        <v>875</v>
       </c>
       <c r="L173" s="25"/>
       <c r="M173" s="25"/>
@@ -13944,7 +13944,7 @@
         <v>848</v>
       </c>
       <c r="K174" s="25" t="s">
-        <v>892</v>
+        <v>875</v>
       </c>
       <c r="L174" s="25"/>
       <c r="M174" s="25"/>
@@ -13982,7 +13982,7 @@
         <v>848</v>
       </c>
       <c r="K175" s="25" t="s">
-        <v>892</v>
+        <v>875</v>
       </c>
       <c r="L175" s="25"/>
       <c r="M175" s="25"/>
@@ -14020,7 +14020,7 @@
         <v>848</v>
       </c>
       <c r="K176" s="25" t="s">
-        <v>896</v>
+        <v>879</v>
       </c>
       <c r="L176" s="25"/>
       <c r="M176" s="25"/>
@@ -14772,7 +14772,7 @@
         <v>848</v>
       </c>
       <c r="K198" s="25" t="s">
-        <v>915</v>
+        <v>898</v>
       </c>
       <c r="L198" s="25"/>
       <c r="M198" s="25"/>
@@ -20790,13 +20790,13 @@
         <v>45265</v>
       </c>
       <c r="G375" s="24" t="s">
-        <v>908</v>
+        <v>891</v>
       </c>
       <c r="H375" s="24" t="s">
-        <v>901</v>
+        <v>884</v>
       </c>
       <c r="I375" s="24" t="s">
-        <v>900</v>
+        <v>883</v>
       </c>
       <c r="J375" s="25" t="s">
         <v>139</v>
@@ -20868,13 +20868,13 @@
         <v>45265</v>
       </c>
       <c r="G377" s="24" t="s">
-        <v>909</v>
+        <v>892</v>
       </c>
       <c r="H377" s="24" t="s">
-        <v>902</v>
+        <v>885</v>
       </c>
       <c r="I377" s="24" t="s">
-        <v>903</v>
+        <v>886</v>
       </c>
       <c r="J377" s="25" t="s">
         <v>139</v>
@@ -21014,13 +21014,13 @@
         <v>45266</v>
       </c>
       <c r="G381" s="24" t="s">
-        <v>912</v>
+        <v>895</v>
       </c>
       <c r="H381" s="24" t="s">
-        <v>913</v>
+        <v>896</v>
       </c>
       <c r="I381" s="24" t="s">
-        <v>914</v>
+        <v>897</v>
       </c>
       <c r="J381" s="25" t="s">
         <v>139</v>
@@ -21096,7 +21096,7 @@
         <v>848</v>
       </c>
       <c r="K383" s="25" t="s">
-        <v>915</v>
+        <v>898</v>
       </c>
       <c r="L383" s="25"/>
       <c r="M383" s="25"/>

</xml_diff>